<commit_message>
Atualiza mapa de fontes
</commit_message>
<xml_diff>
--- a/mapaFontes.xlsx
+++ b/mapaFontes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Documents\GitHub\data_warehouse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadin\Documents\DW\data_warehouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B631762E-8DDA-435D-B966-F9B2F08174B2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2FE6AB-5941-4F3B-89CC-379DBC111ED9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="2" xr2:uid="{4CD9AD75-0ADD-4DE1-8530-2209904B5438}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12168" activeTab="2" xr2:uid="{4CD9AD75-0ADD-4DE1-8530-2209904B5438}"/>
   </bookViews>
   <sheets>
     <sheet name="dimLojaCliente" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="79">
   <si>
     <t>Data Warehouse</t>
   </si>
@@ -110,9 +110,6 @@
     <t>genero</t>
   </si>
   <si>
-    <t>DATE</t>
-  </si>
-  <si>
     <t>Localidade</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>idDimLoja</t>
   </si>
   <si>
-    <t>data_compra</t>
-  </si>
-  <si>
     <t>Loja</t>
   </si>
   <si>
@@ -242,18 +236,9 @@
     <t>calendarioFK</t>
   </si>
   <si>
-    <t>clientes</t>
-  </si>
-  <si>
-    <t>Compra.data_compra</t>
-  </si>
-  <si>
     <t>Compra</t>
   </si>
   <si>
-    <t>data_Compra</t>
-  </si>
-  <si>
     <t>nome cliente</t>
   </si>
   <si>
@@ -266,9 +251,6 @@
     <t>artistas</t>
   </si>
   <si>
-    <t>data</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -276,13 +258,25 @@
   </si>
   <si>
     <t>Compra.custo_toal</t>
+  </si>
+  <si>
+    <t>Calculo da chave de substituição referente à inserção na dimensão disco</t>
+  </si>
+  <si>
+    <t>Calculo da chave de substituição referente à inserção na dimensão loja</t>
+  </si>
+  <si>
+    <t>Calculo da chave de substituição refernete à inserção na dimensão cliente</t>
+  </si>
+  <si>
+    <t>Calculo da chave referente à inserção da data na dimensão calendário</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,6 +286,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -536,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -763,6 +765,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -775,99 +831,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1188,40 +1197,40 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="45.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C2" s="93" t="s">
+    <row r="1" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C2" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="93" t="s">
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="96" t="s">
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="85" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
@@ -1249,14 +1258,14 @@
       <c r="K3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="97"/>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C4" s="86" t="s">
-        <v>58</v>
+      <c r="L3" s="86"/>
+    </row>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C4" s="92" t="s">
+        <v>56</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>12</v>
@@ -1283,149 +1292,149 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C5" s="87"/>
-      <c r="D5" s="90" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="91" t="s">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C5" s="93"/>
+      <c r="D5" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="84" t="s">
+      <c r="F5" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="90" t="s">
         <v>13</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K5" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="91" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="93"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="27" t="s">
         <v>34</v>
-      </c>
-      <c r="L5" s="98" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="87"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="27" t="s">
-        <v>35</v>
       </c>
       <c r="K6" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="98"/>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C7" s="87"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="91"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="84"/>
+      <c r="L6" s="91"/>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C7" s="93"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="90"/>
       <c r="H7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="91"/>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C8" s="92" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="80" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="81" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C9" s="93"/>
+      <c r="D9" s="87" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="88" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="89" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="90" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="27" t="s">
         <v>32</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="72" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" s="98"/>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C8" s="86" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="111" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="112" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C9" s="87"/>
-      <c r="D9" s="90" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="91" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="82" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="84" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>33</v>
       </c>
       <c r="J9" s="27" t="s">
         <v>16</v>
       </c>
       <c r="K9" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" s="89" t="s">
+        <v>33</v>
+      </c>
+      <c r="L9" s="94" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="87"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="91"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="84"/>
+    <row r="10" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="93"/>
+      <c r="D10" s="87"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="90"/>
       <c r="H10" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J10" s="27" t="s">
         <v>16</v>
@@ -1433,273 +1442,273 @@
       <c r="K10" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="89"/>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C11" s="87"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="91"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="84"/>
+      <c r="L10" s="94"/>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C11" s="93"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="90"/>
       <c r="H11" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>14</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="K11" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="89"/>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C12" s="87"/>
-      <c r="D12" s="90" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="91" t="s">
+      <c r="L11" s="94"/>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C12" s="93"/>
+      <c r="D12" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="82" t="s">
+      <c r="F12" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="84" t="s">
+      <c r="G12" s="90" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I12" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="J12" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" s="30" t="s">
+      <c r="L12" s="94" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="93"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" s="27" t="s">
         <v>34</v>
-      </c>
-      <c r="L12" s="89" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="87"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="91"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="84"/>
-      <c r="H13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="J13" s="27" t="s">
-        <v>35</v>
       </c>
       <c r="K13" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="89"/>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C14" s="87"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="91"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="84"/>
+      <c r="L13" s="94"/>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C14" s="93"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="90"/>
       <c r="H14" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>14</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K14" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="89"/>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C15" s="87"/>
-      <c r="D15" s="90" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="91" t="s">
+      <c r="L14" s="94"/>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C15" s="93"/>
+      <c r="D15" s="87" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="82" t="s">
+      <c r="F15" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="84" t="s">
+      <c r="G15" s="90" t="s">
         <v>21</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J15" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="K15" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="L15" s="89" t="s">
+      <c r="L15" s="94" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="87"/>
-      <c r="D16" s="90"/>
-      <c r="E16" s="91"/>
-      <c r="F16" s="82"/>
-      <c r="G16" s="84"/>
+    <row r="16" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="93"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="88"/>
+      <c r="F16" s="89"/>
+      <c r="G16" s="90"/>
       <c r="H16" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J16" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K16" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="89"/>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C17" s="87"/>
-      <c r="D17" s="90"/>
-      <c r="E17" s="91"/>
-      <c r="F17" s="82"/>
-      <c r="G17" s="84"/>
+      <c r="L16" s="94"/>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C17" s="93"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="90"/>
       <c r="H17" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K17" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="89"/>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C18" s="87"/>
-      <c r="D18" s="90" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="91" t="s">
+      <c r="L17" s="94"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="93"/>
+      <c r="D18" s="87" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="82" t="s">
+      <c r="F18" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="84" t="s">
+      <c r="G18" s="90" t="s">
         <v>21</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J18" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K18" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="L18" s="78"/>
-    </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="87"/>
-      <c r="D19" s="90"/>
-      <c r="E19" s="91"/>
-      <c r="F19" s="82"/>
-      <c r="G19" s="84"/>
+      <c r="L18" s="96"/>
+    </row>
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="93"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="89"/>
+      <c r="G19" s="90"/>
       <c r="H19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" s="96"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C20" s="93"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="74" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" s="96"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C21" s="93"/>
+      <c r="D21" s="98" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="89" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="89"/>
+      <c r="G21" s="90"/>
+      <c r="H21" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="J19" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="K19" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L19" s="78"/>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C20" s="87"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="84"/>
-      <c r="H20" s="14" t="s">
+      <c r="I21" s="27" t="s">
         <v>32</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20" s="74" t="s">
-        <v>14</v>
-      </c>
-      <c r="L20" s="78"/>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C21" s="87"/>
-      <c r="D21" s="80" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="82" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="82"/>
-      <c r="G21" s="84"/>
-      <c r="H21" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I21" s="27" t="s">
-        <v>33</v>
       </c>
       <c r="J21" s="27" t="s">
         <v>23</v>
       </c>
       <c r="K21" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="L21" s="78" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="87"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="82"/>
-      <c r="F22" s="82"/>
-      <c r="G22" s="84"/>
+        <v>33</v>
+      </c>
+      <c r="L21" s="96" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="93"/>
+      <c r="D22" s="98"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="89"/>
+      <c r="G22" s="90"/>
       <c r="H22" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J22" s="27" t="s">
         <v>23</v>
@@ -1707,44 +1716,35 @@
       <c r="K22" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="L22" s="78"/>
-    </row>
-    <row r="23" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="88"/>
-      <c r="D23" s="81"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83"/>
-      <c r="G23" s="85"/>
+      <c r="L22" s="96"/>
+    </row>
+    <row r="23" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="95"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="100"/>
+      <c r="F23" s="100"/>
+      <c r="G23" s="101"/>
       <c r="H23" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I23" s="75" t="s">
         <v>14</v>
       </c>
       <c r="J23" s="75" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="K23" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="L23" s="79"/>
+      <c r="L23" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="L5:L7"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="L21:L23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="G21:G23"/>
     <mergeCell ref="C8:C23"/>
     <mergeCell ref="L15:L17"/>
     <mergeCell ref="D18:D20"/>
@@ -1761,11 +1761,20 @@
     <mergeCell ref="E12:E14"/>
     <mergeCell ref="F12:F14"/>
     <mergeCell ref="G12:G14"/>
-    <mergeCell ref="L21:L23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="L5:L7"/>
+    <mergeCell ref="C4:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1779,40 +1788,40 @@
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="45.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="45.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="93" t="s">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="93" t="s">
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="96" t="s">
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="85" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="24" t="s">
         <v>3</v>
       </c>
@@ -1840,14 +1849,14 @@
       <c r="J3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="97"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="105" t="s">
-        <v>56</v>
+      <c r="K3" s="86"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="103" t="s">
+        <v>54</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4" s="39" t="s">
         <v>12</v>
@@ -1874,284 +1883,284 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="106"/>
-      <c r="C5" s="103" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="82" t="s">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="104"/>
+      <c r="C5" s="102" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="84" t="s">
+      <c r="E5" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="90" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="91" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="104"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="98" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="106"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>51</v>
-      </c>
       <c r="I6" s="27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J6" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="98"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="106"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="84"/>
+      <c r="K6" s="91"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="104"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="90"/>
       <c r="G7" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J7" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="98"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="106"/>
-      <c r="C8" s="103" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="82" t="s">
+      <c r="K7" s="91"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="104"/>
+      <c r="C8" s="102" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="84" t="s">
+      <c r="E8" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="90" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J8" s="30" t="s">
         <v>22</v>
       </c>
       <c r="K8" s="22"/>
     </row>
-    <row r="9" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="106"/>
-      <c r="C9" s="103"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="84"/>
+    <row r="9" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="104"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="90"/>
       <c r="G9" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J9" s="30" t="s">
         <v>20</v>
       </c>
       <c r="K9" s="22"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="106"/>
-      <c r="C10" s="103"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="84"/>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="104"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="90"/>
       <c r="G10" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J10" s="30" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K10" s="22"/>
     </row>
-    <row r="11" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="106"/>
-      <c r="C11" s="103" t="s">
+    <row r="11" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="104"/>
+      <c r="C11" s="102" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="89" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="90" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="82" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="84" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="27" t="s">
+      <c r="I11" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="91" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="104"/>
+      <c r="C12" s="102"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="K11" s="98" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="106"/>
-      <c r="C12" s="103"/>
-      <c r="D12" s="82"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="27" t="s">
-        <v>51</v>
-      </c>
       <c r="I12" s="27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J12" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="98"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="106"/>
-      <c r="C13" s="103"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="84"/>
+      <c r="K12" s="91"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="104"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="90"/>
       <c r="G13" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J13" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="98"/>
-    </row>
-    <row r="14" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="106"/>
-      <c r="C14" s="103" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="82" t="s">
+      <c r="K13" s="91"/>
+    </row>
+    <row r="14" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="104"/>
+      <c r="C14" s="102" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="82" t="s">
+      <c r="E14" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="84" t="s">
+      <c r="F14" s="90" t="s">
         <v>21</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H14" s="27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J14" s="30" t="s">
         <v>22</v>
       </c>
       <c r="K14" s="22"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="106"/>
-      <c r="C15" s="103"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="82"/>
-      <c r="F15" s="84"/>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="104"/>
+      <c r="C15" s="102"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="90"/>
       <c r="G15" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H15" s="27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J15" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K15" s="22"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="106"/>
-      <c r="C16" s="103"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="82"/>
-      <c r="F16" s="84"/>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="104"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="90"/>
       <c r="G16" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J16" s="30" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K16" s="22"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="107"/>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="105"/>
       <c r="C17" s="44"/>
       <c r="D17" s="32"/>
       <c r="E17" s="36"/>
@@ -2162,12 +2171,12 @@
       <c r="J17" s="33"/>
       <c r="K17" s="45"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="86" t="s">
-        <v>55</v>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="92" t="s">
+        <v>53</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D18" s="39" t="s">
         <v>12</v>
@@ -2194,62 +2203,62 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="87"/>
-      <c r="C19" s="90" t="s">
+    <row r="19" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="93"/>
+      <c r="C19" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="82" t="s">
+      <c r="D19" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="84" t="s">
+      <c r="E19" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="90" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I19" s="27" t="s">
         <v>24</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="87"/>
-      <c r="C20" s="90"/>
-      <c r="D20" s="82"/>
-      <c r="E20" s="82"/>
-      <c r="F20" s="84"/>
+    <row r="20" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="93"/>
+      <c r="C20" s="87"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="90"/>
       <c r="G20" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H20" s="27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I20" s="27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J20" s="30" t="s">
         <v>20</v>
       </c>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="87"/>
-      <c r="C21" s="90"/>
-      <c r="D21" s="82"/>
-      <c r="E21" s="82"/>
-      <c r="F21" s="84"/>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="93"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="89"/>
+      <c r="E21" s="89"/>
+      <c r="F21" s="90"/>
       <c r="G21" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>14</v>
@@ -2262,42 +2271,42 @@
       </c>
       <c r="K21" s="46"/>
     </row>
-    <row r="22" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="87"/>
-      <c r="C22" s="90" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="82" t="s">
+    <row r="22" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="93"/>
+      <c r="C22" s="87" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="84" t="s">
+      <c r="E22" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="90" t="s">
         <v>13</v>
       </c>
       <c r="G22" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H22" s="27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J22" s="30" t="s">
         <v>12</v>
       </c>
       <c r="K22" s="46"/>
     </row>
-    <row r="23" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="87"/>
-      <c r="C23" s="90"/>
-      <c r="D23" s="82"/>
-      <c r="E23" s="82"/>
-      <c r="F23" s="84"/>
+    <row r="23" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="93"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="90"/>
       <c r="G23" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H23" s="27"/>
       <c r="I23" s="27"/>
@@ -2306,14 +2315,14 @@
       </c>
       <c r="K23" s="46"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="99"/>
-      <c r="C24" s="104"/>
-      <c r="D24" s="100"/>
-      <c r="E24" s="100"/>
-      <c r="F24" s="92"/>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="106"/>
+      <c r="C24" s="107"/>
+      <c r="D24" s="108"/>
+      <c r="E24" s="108"/>
+      <c r="F24" s="111"/>
       <c r="G24" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H24" s="77" t="s">
         <v>14</v>
@@ -2322,12 +2331,12 @@
       <c r="J24" s="33"/>
       <c r="K24" s="48"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="87" t="s">
-        <v>54</v>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="93" t="s">
+        <v>52</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>12</v>
@@ -2354,127 +2363,127 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="87"/>
-      <c r="C26" s="90" t="s">
+    <row r="26" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="93"/>
+      <c r="C26" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="82" t="s">
+      <c r="D26" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="E26" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="84" t="s">
+      <c r="E26" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="90" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H26" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I26" s="49" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J26" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K26" s="35"/>
     </row>
-    <row r="27" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="87"/>
-      <c r="C27" s="90"/>
-      <c r="D27" s="82"/>
-      <c r="E27" s="82"/>
-      <c r="F27" s="84"/>
+    <row r="27" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="93"/>
+      <c r="C27" s="87"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="90"/>
       <c r="G27" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H27" s="27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I27" s="49" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J27" s="50" t="s">
         <v>20</v>
       </c>
       <c r="K27" s="35"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="87"/>
-      <c r="C28" s="90"/>
-      <c r="D28" s="82"/>
-      <c r="E28" s="82"/>
-      <c r="F28" s="84"/>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="93"/>
+      <c r="C28" s="87"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="90"/>
       <c r="G28" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H28" s="71" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I28" s="27" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J28" s="30" t="s">
         <v>20</v>
       </c>
       <c r="K28" s="35"/>
     </row>
-    <row r="29" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="87"/>
-      <c r="C29" s="80" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" s="82" t="s">
+    <row r="29" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="93"/>
+      <c r="C29" s="98" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="101" t="s">
+      <c r="E29" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="109" t="s">
         <v>13</v>
       </c>
       <c r="G29" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H29" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I29" s="27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J29" s="30" t="s">
         <v>12</v>
       </c>
       <c r="K29" s="35"/>
     </row>
-    <row r="30" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="87"/>
-      <c r="C30" s="80"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="82"/>
-      <c r="F30" s="101"/>
+    <row r="30" spans="2:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="93"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="109"/>
       <c r="G30" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H30" s="27"/>
       <c r="I30" s="27"/>
       <c r="J30" s="30"/>
       <c r="K30" s="35"/>
     </row>
-    <row r="31" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="88"/>
-      <c r="C31" s="81"/>
-      <c r="D31" s="83"/>
-      <c r="E31" s="83"/>
-      <c r="F31" s="102"/>
+    <row r="31" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="95"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="100"/>
+      <c r="E31" s="100"/>
+      <c r="F31" s="110"/>
       <c r="G31" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H31" s="75" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I31" s="28"/>
       <c r="J31" s="31"/>
@@ -2482,17 +2491,19 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="K5:K7"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:B17"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="F26:F28"/>
     <mergeCell ref="B25:B31"/>
     <mergeCell ref="B18:B24"/>
     <mergeCell ref="C19:C21"/>
@@ -2509,19 +2520,17 @@
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="C26:C28"/>
     <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="K11:K13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B4:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2530,46 +2539,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7998C3FF-BC13-4892-9A71-4575434B67D1}">
-  <dimension ref="C1:L24"/>
+  <dimension ref="C1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="73.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="73.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C2" s="93" t="s">
+    <row r="1" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C2" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="93" t="s">
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="96" t="s">
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="85" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C3" s="53" t="s">
         <v>3</v>
       </c>
@@ -2597,66 +2606,66 @@
       <c r="K3" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="97"/>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C4" s="105" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="90" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="91" t="s">
+      <c r="L3" s="86"/>
+    </row>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C4" s="103" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="84" t="s">
+      <c r="F4" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="90" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" s="57" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J4" s="57" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K4" s="58" t="s">
         <v>22</v>
       </c>
       <c r="L4" s="60"/>
     </row>
-    <row r="5" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="106"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="84"/>
+    <row r="5" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="104"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="90"/>
       <c r="H5" s="52" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I5" s="57" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J5" s="57" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="K5" s="58" t="s">
         <v>20</v>
       </c>
       <c r="L5" s="60"/>
     </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C6" s="106"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="84"/>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C6" s="104"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="90"/>
       <c r="H6" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>14</v>
@@ -2669,329 +2678,305 @@
       </c>
       <c r="L6" s="60"/>
     </row>
-    <row r="7" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="106"/>
-      <c r="D7" s="90" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="82" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="84" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="52" t="s">
+    <row r="7" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="104"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="22"/>
+    </row>
+    <row r="8" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="104"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="22"/>
+    </row>
+    <row r="9" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="104"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="63"/>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C10" s="104"/>
+      <c r="D10" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="88" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="90" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="78"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="79"/>
+    </row>
+    <row r="11" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="104"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="79"/>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C12" s="104"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="J7" s="62" t="s">
-        <v>72</v>
-      </c>
-      <c r="K7" s="58" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="22"/>
-    </row>
-    <row r="8" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="106"/>
-      <c r="D8" s="90"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="52" t="s">
+      <c r="I12" s="78"/>
+      <c r="J12" s="78"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="79"/>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C13" s="104"/>
+      <c r="D13" s="87" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="90" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="J8" s="62" t="s">
-        <v>70</v>
-      </c>
-      <c r="K8" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="22"/>
-    </row>
-    <row r="9" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="106"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="62" t="s">
-        <v>77</v>
-      </c>
-      <c r="K9" s="58" t="s">
-        <v>25</v>
-      </c>
-      <c r="L9" s="63"/>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C10" s="106"/>
-      <c r="D10" s="90" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="91" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="84" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="60"/>
-    </row>
-    <row r="11" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="106"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="91"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="52" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="60"/>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C12" s="106"/>
-      <c r="D12" s="90"/>
-      <c r="E12" s="91"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="58"/>
-      <c r="L12" s="60"/>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C13" s="106"/>
-      <c r="D13" s="90" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="91" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="84" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="57" t="s">
-        <v>49</v>
-      </c>
-      <c r="J13" s="57" t="s">
+      <c r="I13" s="78" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13" s="78" t="s">
         <v>11</v>
       </c>
       <c r="K13" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="L13" s="108"/>
-    </row>
-    <row r="14" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="106"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="91"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="84"/>
+      <c r="L13" s="114" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="104"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="90"/>
       <c r="H14" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="114"/>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C15" s="104"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="89"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="78"/>
+      <c r="J15" s="78"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="114"/>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C16" s="104"/>
+      <c r="D16" s="87" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="90" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="108"/>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C15" s="106"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="82"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="108"/>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C16" s="106"/>
-      <c r="D16" s="90" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="91" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="84" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="62" t="s">
-        <v>42</v>
-      </c>
-      <c r="J16" s="62" t="s">
+      <c r="I16" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="78" t="s">
         <v>11</v>
       </c>
       <c r="K16" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="109"/>
-    </row>
-    <row r="17" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="106"/>
-      <c r="D17" s="90"/>
-      <c r="E17" s="91"/>
-      <c r="F17" s="82"/>
-      <c r="G17" s="84"/>
+      <c r="L16" s="112" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="104"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="88"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="90"/>
       <c r="H17" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="78"/>
+      <c r="J17" s="78"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="112"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="104"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="78"/>
+      <c r="J18" s="78"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="112"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C19" s="104"/>
+      <c r="D19" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="90" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="58"/>
-      <c r="L17" s="109"/>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C18" s="106"/>
-      <c r="D18" s="90"/>
-      <c r="E18" s="91"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="14" t="s">
+      <c r="I19" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="I18" s="62"/>
-      <c r="J18" s="62"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="109"/>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C19" s="106"/>
-      <c r="D19" s="90" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="91" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="84" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="J19" s="62" t="s">
+      <c r="J19" s="78" t="s">
         <v>11</v>
       </c>
       <c r="K19" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="L19" s="110"/>
-    </row>
-    <row r="20" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="106"/>
-      <c r="D20" s="90"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="84"/>
+      <c r="L19" s="113" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="104"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="88"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="90"/>
       <c r="H20" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="78"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="113"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C21" s="104"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="88"/>
+      <c r="F21" s="89"/>
+      <c r="G21" s="90"/>
+      <c r="H21" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="78"/>
+      <c r="J21" s="78"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="113"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C22" s="104"/>
+      <c r="D22" s="87" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="88" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="89" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="90" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="52" t="s">
         <v>30</v>
-      </c>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="110"/>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C21" s="106"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="91"/>
-      <c r="F21" s="82"/>
-      <c r="G21" s="84"/>
-      <c r="H21" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I21" s="62"/>
-      <c r="J21" s="62"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="110"/>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C22" s="106"/>
-      <c r="D22" s="90" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="91" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="82" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="84" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="52" t="s">
-        <v>31</v>
       </c>
       <c r="I22" s="62"/>
       <c r="J22" s="62"/>
       <c r="K22" s="58"/>
-      <c r="L22" s="78"/>
-    </row>
-    <row r="23" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="106"/>
-      <c r="D23" s="90"/>
-      <c r="E23" s="91"/>
-      <c r="F23" s="82"/>
-      <c r="G23" s="84"/>
+      <c r="L22" s="96" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" s="51" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="104"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="90"/>
       <c r="H23" s="52" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I23" s="62"/>
       <c r="J23" s="62"/>
       <c r="K23" s="58"/>
-      <c r="L23" s="78"/>
-    </row>
-    <row r="24" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L23" s="96"/>
+    </row>
+    <row r="24" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C24" s="69"/>
       <c r="D24" s="65"/>
       <c r="E24" s="70"/>
@@ -3003,16 +2988,22 @@
       <c r="K24" s="59"/>
       <c r="L24" s="61"/>
     </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="F26" s="115"/>
+    </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="D19:D21"/>
     <mergeCell ref="L16:L18"/>
     <mergeCell ref="L19:L21"/>
     <mergeCell ref="L22:L23"/>
@@ -3029,19 +3020,17 @@
     <mergeCell ref="G22:G23"/>
     <mergeCell ref="E19:E21"/>
     <mergeCell ref="F19:F21"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
     <mergeCell ref="L13:L15"/>
-    <mergeCell ref="D22:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>